<commit_message>
Ajout du SWOT dans la SPEC
</commit_message>
<xml_diff>
--- a/LIVRABLE-1/Gestion de projet/SWOT.xlsx
+++ b/LIVRABLE-1/Gestion de projet/SWOT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valentin/Documents/CESI COURS/PFR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain.CHRETIEN\Documents\CESI\snir-co\LIVRABLE-1\Gestion de projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBD88D6C-63B4-8646-A08A-39670D40A61C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553297BF-2717-410E-B902-349669506713}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" xr2:uid="{3BA82F0F-20AA-2B44-912A-E12958777743}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16200" xr2:uid="{3BA82F0F-20AA-2B44-912A-E12958777743}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Forces</t>
   </si>
@@ -45,19 +44,34 @@
     <t>Menaces</t>
   </si>
   <si>
-    <t>Equipe jeune et dynamique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manque d'experience projet </t>
-  </si>
-  <si>
     <t>Conseils de professionnels en entreprise</t>
   </si>
   <si>
     <t xml:space="preserve">Remise des livrables dans les temps avec les differents projets à rendre (entreprise) </t>
   </si>
   <si>
-    <t>Durée du projet</t>
+    <t xml:space="preserve">Concurrence et futur évolutions </t>
+  </si>
+  <si>
+    <t>Connaissances fonctionnelles du BTP</t>
+  </si>
+  <si>
+    <t>Equipe dynamique</t>
+  </si>
+  <si>
+    <t>Equipe toujours en veille technologique</t>
+  </si>
+  <si>
+    <t>Augmenter l'image de marque de la société</t>
+  </si>
+  <si>
+    <t>Acquerir de l"experience dans le domaine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efficacité de réaction face à l'imprévu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manque d'experience de projet </t>
   </si>
 </sst>
 </file>
@@ -152,30 +166,30 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -493,127 +507,128 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5B3FE4-B6D5-0543-96AD-4637C385891D}">
   <dimension ref="B1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:G4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
-    <col min="7" max="7" width="27.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.296875" customWidth="1"/>
+    <col min="5" max="5" width="14.796875" customWidth="1"/>
+    <col min="7" max="7" width="27.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+    <row r="1" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="7" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="4" t="s">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="5" t="s">
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E8:G9"/>
@@ -624,6 +639,15 @@
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>